<commit_message>
Added some analysis into the formatted files
</commit_message>
<xml_diff>
--- a/results/results_formatted/evaluation_freeRoaming20_run1_formatted.xlsx
+++ b/results/results_formatted/evaluation_freeRoaming20_run1_formatted.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamza\Desktop\bro usb n papa\results (free roaming)\editted\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaZa\Music\APP-RAS paper results\analysis\results (free roaming)\formatted\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7652AA9-E6CA-44FC-A4EA-CC7401974A63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evaluation_freeRoaming20_run1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="29">
   <si>
     <t>charging</t>
   </si>
@@ -92,11 +101,26 @@
   <si>
     <t>Final Battery level (battery when task finished)</t>
   </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Waiting Time</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Charging</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,8 +437,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -529,6 +559,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -574,9 +619,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -897,29 +948,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="H154" sqref="H154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -960,7 +1011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -992,7 +1043,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1075,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1065,7 +1116,7 @@
         <v>57.71</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1106,7 +1157,7 @@
         <v>54.77</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1147,7 +1198,7 @@
         <v>53.95</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1188,7 +1239,7 @@
         <v>59.81</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1280,7 @@
         <v>56.09</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1270,7 +1321,7 @@
         <v>69.650000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1311,7 +1362,7 @@
         <v>77.599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1352,7 +1403,7 @@
         <v>35.630000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1393,7 +1444,7 @@
         <v>27.48</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1434,7 +1485,7 @@
         <v>37.159999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1475,7 +1526,7 @@
         <v>28.73</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1516,7 +1567,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1608,7 @@
         <v>29.78</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1598,7 +1649,7 @@
         <v>49.81</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1639,7 +1690,7 @@
         <v>19.47</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1722,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1712,7 +1763,7 @@
         <v>46.26</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -1753,7 +1804,7 @@
         <v>20.04</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -1794,7 +1845,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1877,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1867,7 +1918,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1908,7 +1959,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1940,7 +1991,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1981,7 +2032,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -2022,7 +2073,7 @@
         <v>10.16</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2105,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -2095,7 +2146,7 @@
         <v>66.069999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2136,7 +2187,7 @@
         <v>73.84</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2168,7 +2219,7 @@
         <v>29.55</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2200,7 +2251,7 @@
         <v>26.35</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2232,7 +2283,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
@@ -2273,7 +2324,7 @@
         <v>71.98</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2305,7 +2356,7 @@
         <v>28.26</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -2346,7 +2397,7 @@
         <v>80.81</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -2387,7 +2438,7 @@
         <v>35.81</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -2428,7 +2479,7 @@
         <v>42.31</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -2469,7 +2520,7 @@
         <v>38.909999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -2510,7 +2561,7 @@
         <v>61.01</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>3</v>
       </c>
@@ -2551,7 +2602,7 @@
         <v>69.52</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -2592,7 +2643,7 @@
         <v>78.7</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>3</v>
       </c>
@@ -2633,7 +2684,7 @@
         <v>56.55</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2674,7 +2725,7 @@
         <v>27.72</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -2715,7 +2766,7 @@
         <v>40.869999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -2756,7 +2807,7 @@
         <v>19.23</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -2797,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -2838,7 +2889,7 @@
         <v>37.75</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -2879,7 +2930,7 @@
         <v>28.12</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -2920,7 +2971,7 @@
         <v>36.69</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -2961,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -2993,7 +3044,7 @@
         <v>25.44</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -3025,7 +3076,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>3</v>
       </c>
@@ -3066,7 +3117,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
@@ -3107,7 +3158,7 @@
         <v>10.38</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -3139,7 +3190,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
@@ -3180,7 +3231,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>3</v>
       </c>
@@ -3221,7 +3272,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
@@ -3262,7 +3313,7 @@
         <v>71.41</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -3294,7 +3345,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>3</v>
       </c>
@@ -3335,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>3</v>
       </c>
@@ -3376,7 +3427,7 @@
         <v>70.78</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -3408,7 +3459,7 @@
         <v>27.55</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -3440,7 +3491,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
@@ -3481,7 +3532,7 @@
         <v>69.41</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -3513,7 +3564,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -3554,7 +3605,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>3</v>
       </c>
@@ -3595,7 +3646,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
@@ -3636,7 +3687,7 @@
         <v>27.83</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>3</v>
       </c>
@@ -3677,7 +3728,7 @@
         <v>72.37</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>3</v>
       </c>
@@ -3718,7 +3769,7 @@
         <v>41.94</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>3</v>
       </c>
@@ -3759,7 +3810,7 @@
         <v>68.14</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
@@ -3800,7 +3851,7 @@
         <v>78.97</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>3</v>
       </c>
@@ -3841,7 +3892,7 @@
         <v>27.34</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
@@ -3882,7 +3933,7 @@
         <v>4.92</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>3</v>
       </c>
@@ -3923,7 +3974,7 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -3955,7 +4006,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>3</v>
       </c>
@@ -3996,7 +4047,7 @@
         <v>8.2799999999999994</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>3</v>
       </c>
@@ -4037,7 +4088,7 @@
         <v>32.07</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
@@ -4078,7 +4129,7 @@
         <v>51.73</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -4110,7 +4161,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -4142,7 +4193,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -4174,7 +4225,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>3</v>
       </c>
@@ -4215,7 +4266,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>3</v>
       </c>
@@ -4256,7 +4307,7 @@
         <v>19.72</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>3</v>
       </c>
@@ -4297,7 +4348,7 @@
         <v>9.59</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>3</v>
       </c>
@@ -4338,7 +4389,7 @@
         <v>27.41</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>3</v>
       </c>
@@ -4379,7 +4430,7 @@
         <v>68.31</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -4411,7 +4462,7 @@
         <v>27.65</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>3</v>
       </c>
@@ -4452,7 +4503,7 @@
         <v>62.29</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>3</v>
       </c>
@@ -4493,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>3</v>
       </c>
@@ -4534,7 +4585,7 @@
         <v>8.3699999999999992</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>3</v>
       </c>
@@ -4575,7 +4626,7 @@
         <v>20.62</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>3</v>
       </c>
@@ -4616,7 +4667,7 @@
         <v>34.42</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>3</v>
       </c>
@@ -4657,7 +4708,7 @@
         <v>36.659999999999997</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -4689,7 +4740,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -4721,7 +4772,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>3</v>
       </c>
@@ -4762,7 +4813,7 @@
         <v>65.760000000000005</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>3</v>
       </c>
@@ -4803,7 +4854,7 @@
         <v>16.87</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -4835,7 +4886,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>3</v>
       </c>
@@ -4876,7 +4927,7 @@
         <v>11.68</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>3</v>
       </c>
@@ -4917,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -4949,7 +5000,7 @@
         <v>25.65</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>3</v>
       </c>
@@ -4990,7 +5041,7 @@
         <v>42.91</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>3</v>
       </c>
@@ -5031,7 +5082,7 @@
         <v>60.35</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>3</v>
       </c>
@@ -5072,7 +5123,7 @@
         <v>68.37</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>0</v>
       </c>
@@ -5104,7 +5155,7 @@
         <v>30.05</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>3</v>
       </c>
@@ -5145,7 +5196,7 @@
         <v>5.14</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>3</v>
       </c>
@@ -5186,7 +5237,7 @@
         <v>70.39</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>3</v>
       </c>
@@ -5227,7 +5278,7 @@
         <v>38.07</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>3</v>
       </c>
@@ -5268,7 +5319,7 @@
         <v>37.54</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
@@ -5309,7 +5360,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
@@ -5341,7 +5392,7 @@
         <v>27.65</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>3</v>
       </c>
@@ -5382,7 +5433,7 @@
         <v>62.94</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>3</v>
       </c>
@@ -5423,7 +5474,7 @@
         <v>40.08</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>3</v>
       </c>
@@ -5464,7 +5515,7 @@
         <v>14.49</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -5496,7 +5547,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>3</v>
       </c>
@@ -5537,7 +5588,7 @@
         <v>75.650000000000006</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>3</v>
       </c>
@@ -5578,7 +5629,7 @@
         <v>5.22</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>3</v>
       </c>
@@ -5619,7 +5670,7 @@
         <v>13.65</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
@@ -5660,7 +5711,7 @@
         <v>69.069999999999993</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>3</v>
       </c>
@@ -5701,7 +5752,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>3</v>
       </c>
@@ -5742,7 +5793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>3</v>
       </c>
@@ -5783,7 +5834,7 @@
         <v>46.38</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
@@ -5815,7 +5866,7 @@
         <v>29.05</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -5847,7 +5898,7 @@
         <v>29.65</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>3</v>
       </c>
@@ -5888,7 +5939,7 @@
         <v>45.42</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>3</v>
       </c>
@@ -5929,7 +5980,7 @@
         <v>4.38</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -5961,7 +6012,7 @@
         <v>28.65</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
@@ -6002,7 +6053,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>3</v>
       </c>
@@ -6043,7 +6094,7 @@
         <v>75.83</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -6075,7 +6126,7 @@
         <v>30.7</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>3</v>
       </c>
@@ -6116,7 +6167,7 @@
         <v>58.04</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>3</v>
       </c>
@@ -6157,7 +6208,7 @@
         <v>64.989999999999995</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>3</v>
       </c>
@@ -6198,7 +6249,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>0</v>
       </c>
@@ -6230,7 +6281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>3</v>
       </c>
@@ -6271,7 +6322,7 @@
         <v>56.03</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>3</v>
       </c>
@@ -6312,7 +6363,7 @@
         <v>58.46</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>3</v>
       </c>
@@ -6353,7 +6404,7 @@
         <v>26.53</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>0</v>
       </c>
@@ -6385,7 +6436,7 @@
         <v>30.85</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>10</v>
       </c>
@@ -6396,7 +6447,7 @@
         <v>379.45</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>10</v>
       </c>
@@ -6407,7 +6458,7 @@
         <v>304.52</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>10</v>
       </c>
@@ -6418,7 +6469,7 @@
         <v>378.7</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>10</v>
       </c>
@@ -6429,7 +6480,7 @@
         <v>284.58</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>10</v>
       </c>
@@ -6440,7 +6491,7 @@
         <v>93.96</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>10</v>
       </c>
@@ -6451,7 +6502,7 @@
         <v>386.43</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>10</v>
       </c>
@@ -6462,7 +6513,7 @@
         <v>335.88</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>10</v>
       </c>
@@ -6471,6 +6522,54 @@
       </c>
       <c r="C149">
         <v>432.41</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E151" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E152" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F152" s="3">
+        <f>COUNTIF(A2:A141,"transportation")</f>
+        <v>105</v>
+      </c>
+      <c r="G152" s="3">
+        <f>AVERAGEIF(A2:A141,"transportation",F2:F141)</f>
+        <v>141.43219047619053</v>
+      </c>
+      <c r="H152" s="3">
+        <f>AVERAGEIF(A2:A141,"transportation",H2:H141)</f>
+        <v>79.132952380952361</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E153" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F153" s="3">
+        <f>COUNTIF(A2:A141,"charging")</f>
+        <v>35</v>
+      </c>
+      <c r="G153" s="3">
+        <f>AVERAGEIF(A2:A141,"charging",F2:F141)</f>
+        <v>42.90971428571428</v>
+      </c>
+      <c r="H153" s="3">
+        <f>AVERAGEIF(A2:A141,"charging",H2:H141)</f>
+        <v>0.29857142857142854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>